<commit_message>
fix import add condition on null
</commit_message>
<xml_diff>
--- a/public/excel/import.xlsx
+++ b/public/excel/import.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -336,7 +336,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -347,7 +347,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>